<commit_message>
basic us gdp fert
</commit_message>
<xml_diff>
--- a/data/WDI_Data.csv.xlsx
+++ b/data/WDI_Data.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njayj\WebstormProjects\vega1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8A6DDF-801A-4FC5-981B-CA9CB65C3389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DADA74-EE81-4F59-93FC-E582631526FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AE4DB062-F6F2-43E3-B434-690B406A895F}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{AE4DB062-F6F2-43E3-B434-690B406A895F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,7 +445,7 @@
     <col min="2" max="2" width="17.54296875" customWidth="1"/>
     <col min="3" max="3" width="38.08984375" customWidth="1"/>
     <col min="4" max="4" width="36.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="28.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>